<commit_message>
TestPlan and blackbox testing updated
</commit_message>
<xml_diff>
--- a/BlackBoxTest.xlsx
+++ b/BlackBoxTest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\SD6503_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96C953B2-E6FF-430F-BD8C-8DA199ABE398}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ECB5844-B92A-42EB-8F9D-67990A8ABCDC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{29A32F6C-B3F9-4A8E-A7D7-18A440C3D2C0}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="151">
   <si>
     <t>BLACK BOX TESTING</t>
   </si>
@@ -462,6 +462,36 @@
   </si>
   <si>
     <t>The page redirects to the statistics index page with the saved info</t>
+  </si>
+  <si>
+    <t>Search Functionality</t>
+  </si>
+  <si>
+    <t>A new team has been created</t>
+  </si>
+  <si>
+    <t>Type data in the textbox and press search button</t>
+  </si>
+  <si>
+    <t>The page loads information that matches the search input</t>
+  </si>
+  <si>
+    <t>One Click on the name title/tab you want to sort by.</t>
+  </si>
+  <si>
+    <t>The page sorts in ascending order of team name.</t>
+  </si>
+  <si>
+    <t>Sort Functionality (Ascending)</t>
+  </si>
+  <si>
+    <t>Sort Functionality (Descending)</t>
+  </si>
+  <si>
+    <t>Double Click on the name title/tab you want to sort by.</t>
+  </si>
+  <si>
+    <t>The page sorts in descending order of team name.</t>
   </si>
 </sst>
 </file>
@@ -851,7 +881,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -919,18 +949,54 @@
     <xf numFmtId="0" fontId="11" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -951,36 +1017,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1297,10 +1333,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F709F99-23DD-449C-B30A-BC06EF912437}">
-  <dimension ref="B1:I61"/>
+  <dimension ref="B1:I67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H60" sqref="H60"/>
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1309,32 +1345,32 @@
     <col min="3" max="3" width="16.140625" customWidth="1"/>
     <col min="4" max="4" width="18.140625" customWidth="1"/>
     <col min="5" max="5" width="25.85546875" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" customWidth="1"/>
+    <col min="6" max="6" width="18.7109375" customWidth="1"/>
     <col min="7" max="7" width="19.85546875" customWidth="1"/>
     <col min="8" max="8" width="19.140625" customWidth="1"/>
     <col min="9" max="9" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D1" s="36" t="s">
+      <c r="D1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="38"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="33"/>
     </row>
     <row r="2" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="2:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="27"/>
-      <c r="H3" s="27"/>
-      <c r="I3" s="28"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="40"/>
     </row>
     <row r="4" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="22" t="s">
@@ -1425,16 +1461,16 @@
       <c r="I7" s="5"/>
     </row>
     <row r="8" spans="2:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="26" t="s">
+      <c r="B8" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="39"/>
-      <c r="D8" s="39"/>
-      <c r="E8" s="39"/>
-      <c r="F8" s="39"/>
-      <c r="G8" s="39"/>
-      <c r="H8" s="39"/>
-      <c r="I8" s="40"/>
+      <c r="C8" s="35"/>
+      <c r="D8" s="35"/>
+      <c r="E8" s="35"/>
+      <c r="F8" s="35"/>
+      <c r="G8" s="35"/>
+      <c r="H8" s="35"/>
+      <c r="I8" s="36"/>
     </row>
     <row r="9" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="20" t="s">
@@ -1489,40 +1525,40 @@
       </c>
     </row>
     <row r="11" spans="2:9" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="34" t="s">
+      <c r="B11" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="34" t="s">
+      <c r="C11" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="D11" s="34" t="s">
-        <v>9</v>
-      </c>
-      <c r="E11" s="34" t="s">
+      <c r="D11" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="F11" s="34" t="s">
+      <c r="F11" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="G11" s="34" t="s">
+      <c r="G11" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="H11" s="34" t="s">
+      <c r="H11" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="I11" s="34" t="s">
+      <c r="I11" s="29" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B12" s="35"/>
-      <c r="C12" s="35"/>
-      <c r="D12" s="35"/>
-      <c r="E12" s="35"/>
-      <c r="F12" s="35"/>
-      <c r="G12" s="35"/>
-      <c r="H12" s="35"/>
-      <c r="I12" s="35"/>
+      <c r="B12" s="30"/>
+      <c r="C12" s="30"/>
+      <c r="D12" s="30"/>
+      <c r="E12" s="30"/>
+      <c r="F12" s="30"/>
+      <c r="G12" s="30"/>
+      <c r="H12" s="30"/>
+      <c r="I12" s="30"/>
     </row>
     <row r="13" spans="2:9" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="9" t="s">
@@ -1550,331 +1586,331 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="2:9" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="34" t="s">
+    <row r="14" spans="2:9" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="23" t="s">
+        <v>141</v>
+      </c>
+      <c r="C14" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="F14" s="24" t="s">
+        <v>143</v>
+      </c>
+      <c r="G14" s="23" t="s">
+        <v>144</v>
+      </c>
+      <c r="H14" s="23" t="s">
+        <v>144</v>
+      </c>
+      <c r="I14" s="23" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="23" t="s">
+        <v>147</v>
+      </c>
+      <c r="C15" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="F15" s="24" t="s">
+        <v>145</v>
+      </c>
+      <c r="G15" s="23" t="s">
+        <v>146</v>
+      </c>
+      <c r="H15" s="23" t="s">
+        <v>146</v>
+      </c>
+      <c r="I15" s="23" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="23" t="s">
+        <v>148</v>
+      </c>
+      <c r="C16" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="D16" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="F16" s="24" t="s">
+        <v>149</v>
+      </c>
+      <c r="G16" s="23" t="s">
+        <v>150</v>
+      </c>
+      <c r="H16" s="23" t="s">
+        <v>150</v>
+      </c>
+      <c r="I16" s="23" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="34" t="s">
-        <v>36</v>
-      </c>
-      <c r="D14" s="34" t="s">
-        <v>9</v>
-      </c>
-      <c r="E14" s="34" t="s">
+      <c r="C17" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="D17" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="F14" s="34" t="s">
+      <c r="F17" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="G14" s="34" t="s">
+      <c r="G17" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="H14" s="34" t="s">
+      <c r="H17" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="I14" s="34" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B15" s="35"/>
-      <c r="C15" s="35"/>
-      <c r="D15" s="35"/>
-      <c r="E15" s="35"/>
-      <c r="F15" s="35"/>
-      <c r="G15" s="35"/>
-      <c r="H15" s="35"/>
-      <c r="I15" s="35"/>
-    </row>
-    <row r="16" spans="2:9" ht="57" x14ac:dyDescent="0.25">
-      <c r="B16" s="11" t="s">
+      <c r="I17" s="29" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B18" s="30"/>
+      <c r="C18" s="30"/>
+      <c r="D18" s="30"/>
+      <c r="E18" s="30"/>
+      <c r="F18" s="30"/>
+      <c r="G18" s="30"/>
+      <c r="H18" s="30"/>
+      <c r="I18" s="30"/>
+    </row>
+    <row r="19" spans="2:9" ht="57" x14ac:dyDescent="0.25">
+      <c r="B19" s="11" t="s">
         <v>127</v>
       </c>
-      <c r="C16" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="D16" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="E16" s="11" t="s">
+      <c r="C19" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" s="11" t="s">
         <v>128</v>
       </c>
-      <c r="F16" s="11" t="s">
+      <c r="F19" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="G16" s="11" t="s">
+      <c r="G19" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="H16" s="11" t="s">
+      <c r="H19" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="I16" s="11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="2:9" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="34" t="s">
+      <c r="I19" s="11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="C17" s="34" t="s">
-        <v>45</v>
-      </c>
-      <c r="D17" s="34" t="s">
-        <v>9</v>
-      </c>
-      <c r="E17" s="34" t="s">
+      <c r="C20" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="D20" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="F17" s="34" t="s">
+      <c r="F20" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="G17" s="34" t="s">
+      <c r="G20" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="H17" s="34" t="s">
+      <c r="H20" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="I17" s="34" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B18" s="34"/>
-      <c r="C18" s="34"/>
-      <c r="D18" s="34"/>
-      <c r="E18" s="34"/>
-      <c r="F18" s="34"/>
-      <c r="G18" s="34"/>
-      <c r="H18" s="34"/>
-      <c r="I18" s="34"/>
-    </row>
-    <row r="19" spans="2:9" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="34" t="s">
+      <c r="I20" s="29" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B21" s="29"/>
+      <c r="C21" s="29"/>
+      <c r="D21" s="29"/>
+      <c r="E21" s="29"/>
+      <c r="F21" s="29"/>
+      <c r="G21" s="29"/>
+      <c r="H21" s="29"/>
+      <c r="I21" s="29"/>
+    </row>
+    <row r="22" spans="2:9" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="C19" s="34" t="s">
-        <v>50</v>
-      </c>
-      <c r="D19" s="34" t="s">
-        <v>9</v>
-      </c>
-      <c r="E19" s="34" t="s">
+      <c r="C22" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="D22" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="E22" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="F19" s="34" t="s">
+      <c r="F22" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="G19" s="34" t="s">
+      <c r="G22" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="H19" s="34" t="s">
+      <c r="H22" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="I19" s="34" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B20" s="34"/>
-      <c r="C20" s="34"/>
-      <c r="D20" s="34"/>
-      <c r="E20" s="34"/>
-      <c r="F20" s="34"/>
-      <c r="G20" s="34"/>
-      <c r="H20" s="34"/>
-      <c r="I20" s="34"/>
-    </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B21" s="4"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
-      <c r="I21" s="5"/>
-    </row>
-    <row r="22" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="4"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="5"/>
-    </row>
-    <row r="23" spans="2:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="29" t="s">
+      <c r="I22" s="29" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B23" s="29"/>
+      <c r="C23" s="29"/>
+      <c r="D23" s="29"/>
+      <c r="E23" s="29"/>
+      <c r="F23" s="29"/>
+      <c r="G23" s="29"/>
+      <c r="H23" s="29"/>
+      <c r="I23" s="29"/>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B24" s="4"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="5"/>
+    </row>
+    <row r="25" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="4"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="5"/>
+    </row>
+    <row r="26" spans="2:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B26" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="C23" s="32"/>
-      <c r="D23" s="32"/>
-      <c r="E23" s="32"/>
-      <c r="F23" s="32"/>
-      <c r="G23" s="32"/>
-      <c r="H23" s="32"/>
-      <c r="I23" s="33"/>
-    </row>
-    <row r="24" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="20" t="s">
+      <c r="C26" s="44"/>
+      <c r="D26" s="44"/>
+      <c r="E26" s="44"/>
+      <c r="F26" s="44"/>
+      <c r="G26" s="44"/>
+      <c r="H26" s="44"/>
+      <c r="I26" s="45"/>
+    </row>
+    <row r="27" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C24" s="20" t="s">
+      <c r="C27" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D24" s="20" t="s">
+      <c r="D27" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E24" s="20" t="s">
+      <c r="E27" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="F24" s="20" t="s">
+      <c r="F27" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="G24" s="20" t="s">
+      <c r="G27" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="H24" s="20" t="s">
+      <c r="H27" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="I24" s="21" t="s">
+      <c r="I27" s="21" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="2:9" ht="57" x14ac:dyDescent="0.25">
-      <c r="B25" s="10" t="s">
+    <row r="28" spans="2:9" ht="57" x14ac:dyDescent="0.25">
+      <c r="B28" s="10" t="s">
         <v>58</v>
-      </c>
-      <c r="C25" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="D25" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E25" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="F25" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="G25" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="H25" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="I25" s="7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="26" spans="2:9" ht="85.5" x14ac:dyDescent="0.25">
-      <c r="B26" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="C26" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="D26" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E26" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="F26" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="G26" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="H26" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="I26" s="9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="27" spans="2:9" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="C27" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="D27" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E27" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="F27" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="G27" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="H27" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="I27" s="9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="28" spans="2:9" ht="71.25" x14ac:dyDescent="0.25">
-      <c r="B28" s="9" t="s">
-        <v>43</v>
       </c>
       <c r="C28" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="D28" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E28" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="F28" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="G28" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="H28" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="I28" s="9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="29" spans="2:9" ht="57" x14ac:dyDescent="0.25">
-      <c r="B29" s="11" t="s">
-        <v>127</v>
+      <c r="D28" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E28" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F28" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="G28" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="H28" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="I28" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" ht="85.5" x14ac:dyDescent="0.25">
+      <c r="B29" s="9" t="s">
+        <v>35</v>
       </c>
       <c r="C29" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="D29" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="E29" s="11" t="s">
-        <v>128</v>
-      </c>
-      <c r="F29" s="11" t="s">
-        <v>129</v>
-      </c>
-      <c r="G29" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="H29" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="I29" s="11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="30" spans="2:9" ht="85.5" x14ac:dyDescent="0.25">
+      <c r="D29" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E29" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="F29" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G29" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="H29" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="I29" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="9" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="C30" s="10" t="s">
         <v>72</v>
@@ -1883,726 +1919,881 @@
         <v>9</v>
       </c>
       <c r="E30" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="F30" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="G30" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="H30" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="I30" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="23" t="s">
+        <v>141</v>
+      </c>
+      <c r="C31" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="D31" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="E31" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="F31" s="24" t="s">
+        <v>143</v>
+      </c>
+      <c r="G31" s="23" t="s">
+        <v>144</v>
+      </c>
+      <c r="H31" s="23" t="s">
+        <v>144</v>
+      </c>
+      <c r="I31" s="23" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="23" t="s">
+        <v>147</v>
+      </c>
+      <c r="C32" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="D32" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="E32" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="F32" s="24" t="s">
+        <v>145</v>
+      </c>
+      <c r="G32" s="23" t="s">
+        <v>146</v>
+      </c>
+      <c r="H32" s="23" t="s">
+        <v>146</v>
+      </c>
+      <c r="I32" s="23" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="23" t="s">
+        <v>148</v>
+      </c>
+      <c r="C33" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="D33" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="E33" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="F33" s="24" t="s">
+        <v>149</v>
+      </c>
+      <c r="G33" s="23" t="s">
+        <v>150</v>
+      </c>
+      <c r="H33" s="23" t="s">
+        <v>150</v>
+      </c>
+      <c r="I33" s="23" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9" ht="71.25" x14ac:dyDescent="0.25">
+      <c r="B34" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C34" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E34" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="F34" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="G34" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="H34" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="I34" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="2:9" ht="57" x14ac:dyDescent="0.25">
+      <c r="B35" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="D35" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E35" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="F35" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="G35" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="H35" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="I35" s="11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="2:9" ht="71.25" x14ac:dyDescent="0.25">
+      <c r="B36" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C36" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="D36" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E36" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="F30" s="9" t="s">
+      <c r="F36" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="G30" s="9" t="s">
+      <c r="G36" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="H30" s="9" t="s">
+      <c r="H36" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="I30" s="9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="31" spans="2:9" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="9" t="s">
+      <c r="I36" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="2:9" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="C31" s="10" t="s">
+      <c r="C37" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="D31" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E31" s="9" t="s">
+      <c r="D37" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E37" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="F31" s="9" t="s">
+      <c r="F37" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="G31" s="9" t="s">
+      <c r="G37" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="H31" s="9" t="s">
+      <c r="H37" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="I31" s="9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="32" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="33" spans="2:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B33" s="29" t="s">
+      <c r="I37" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="39" spans="2:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B39" s="41" t="s">
         <v>71</v>
       </c>
-      <c r="C33" s="30"/>
-      <c r="D33" s="30"/>
-      <c r="E33" s="30"/>
-      <c r="F33" s="30"/>
-      <c r="G33" s="30"/>
-      <c r="H33" s="30"/>
-      <c r="I33" s="31"/>
-    </row>
-    <row r="34" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="22" t="s">
+      <c r="C39" s="42"/>
+      <c r="D39" s="42"/>
+      <c r="E39" s="42"/>
+      <c r="F39" s="42"/>
+      <c r="G39" s="42"/>
+      <c r="H39" s="42"/>
+      <c r="I39" s="43"/>
+    </row>
+    <row r="40" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B40" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C34" s="22" t="s">
+      <c r="C40" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="D34" s="22" t="s">
+      <c r="D40" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="E34" s="22" t="s">
+      <c r="E40" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="F34" s="22" t="s">
+      <c r="F40" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="G34" s="22" t="s">
+      <c r="G40" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="H34" s="22" t="s">
+      <c r="H40" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="I34" s="21" t="s">
+      <c r="I40" s="21" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="2:9" ht="57" x14ac:dyDescent="0.25">
-      <c r="B35" s="18" t="s">
+    <row r="41" spans="2:9" ht="57" x14ac:dyDescent="0.25">
+      <c r="B41" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="C35" s="18" t="s">
+      <c r="C41" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="D35" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="E35" s="18" t="s">
+      <c r="D41" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="E41" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="F35" s="18" t="s">
+      <c r="F41" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="G35" s="18" t="s">
+      <c r="G41" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="H35" s="18" t="s">
+      <c r="H41" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="I35" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="36" spans="2:9" ht="114" x14ac:dyDescent="0.25">
-      <c r="B36" s="13" t="s">
+      <c r="I41" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="42" spans="2:9" ht="114" x14ac:dyDescent="0.25">
+      <c r="B42" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="C36" s="18" t="s">
+      <c r="C42" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="D36" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="E36" s="13" t="s">
+      <c r="D42" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="E42" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="F36" s="13" t="s">
+      <c r="F42" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="G36" s="13" t="s">
+      <c r="G42" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="H36" s="14" t="s">
+      <c r="H42" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="I36" s="8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="37" spans="2:9" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="3" t="s">
+      <c r="I42" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43" spans="2:9" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C37" s="18" t="s">
+      <c r="C43" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="D37" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="E37" s="3" t="s">
+      <c r="D43" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E43" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="F37" s="3" t="s">
+      <c r="F43" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="G37" s="3" t="s">
+      <c r="G43" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="H37" s="3" t="s">
+      <c r="H43" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="I37" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="38" spans="2:9" ht="57" x14ac:dyDescent="0.25">
-      <c r="B38" s="12" t="s">
+      <c r="I43" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="44" spans="2:9" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B44" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="C38" s="18" t="s">
+      <c r="C44" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="D38" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E38" s="16" t="s">
+      <c r="D44" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E44" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="F38" s="12" t="s">
+      <c r="F44" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="G38" s="12" t="s">
+      <c r="G44" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="H38" s="17" t="s">
+      <c r="H44" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="I38" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="39" spans="2:9" ht="57" x14ac:dyDescent="0.25">
-      <c r="B39" s="11" t="s">
+      <c r="I44" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="45" spans="2:9" ht="57" x14ac:dyDescent="0.25">
+      <c r="B45" s="11" t="s">
         <v>127</v>
       </c>
-      <c r="C39" s="10" t="s">
+      <c r="C45" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="D39" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="E39" s="11" t="s">
+      <c r="D45" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E45" s="11" t="s">
         <v>128</v>
       </c>
-      <c r="F39" s="11" t="s">
+      <c r="F45" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="G39" s="11" t="s">
+      <c r="G45" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="H39" s="11" t="s">
+      <c r="H45" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="I39" s="11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="40" spans="2:9" ht="110.25" x14ac:dyDescent="0.25">
-      <c r="B40" s="12" t="s">
+      <c r="I45" s="11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="46" spans="2:9" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="B46" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="C40" s="10" t="s">
+      <c r="C46" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="D40" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E40" s="16" t="s">
+      <c r="D46" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E46" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="F40" s="12" t="s">
+      <c r="F46" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="G40" s="12" t="s">
+      <c r="G46" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="H40" s="17" t="s">
+      <c r="H46" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="I40" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="41" spans="2:9" ht="110.25" x14ac:dyDescent="0.25">
-      <c r="B41" s="12" t="s">
+      <c r="I46" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="47" spans="2:9" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="B47" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="C41" s="10" t="s">
+      <c r="C47" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="D41" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E41" s="16" t="s">
+      <c r="D47" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E47" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="F41" s="12" t="s">
+      <c r="F47" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="G41" s="12" t="s">
+      <c r="G47" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="H41" s="17" t="s">
+      <c r="H47" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="I41" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="42" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="43" spans="2:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B43" s="23" t="s">
+      <c r="I47" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="48" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="49" spans="2:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B49" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="C43" s="24"/>
-      <c r="D43" s="24"/>
-      <c r="E43" s="24"/>
-      <c r="F43" s="24"/>
-      <c r="G43" s="24"/>
-      <c r="H43" s="24"/>
-      <c r="I43" s="25"/>
-    </row>
-    <row r="44" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="22" t="s">
+      <c r="C49" s="37"/>
+      <c r="D49" s="37"/>
+      <c r="E49" s="37"/>
+      <c r="F49" s="37"/>
+      <c r="G49" s="37"/>
+      <c r="H49" s="37"/>
+      <c r="I49" s="38"/>
+    </row>
+    <row r="50" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B50" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C44" s="22" t="s">
+      <c r="C50" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="D44" s="22" t="s">
+      <c r="D50" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="E44" s="22" t="s">
+      <c r="E50" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="F44" s="22" t="s">
+      <c r="F50" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="G44" s="22" t="s">
+      <c r="G50" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="H44" s="22" t="s">
+      <c r="H50" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="I44" s="21" t="s">
+      <c r="I50" s="21" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="45" spans="2:9" ht="57" x14ac:dyDescent="0.25">
-      <c r="B45" s="6" t="s">
+    <row r="51" spans="2:9" ht="57" x14ac:dyDescent="0.25">
+      <c r="B51" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="C45" s="6" t="s">
+      <c r="C51" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="D45" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E45" s="6" t="s">
+      <c r="D51" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E51" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F45" s="6" t="s">
+      <c r="F51" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="G45" s="6" t="s">
+      <c r="G51" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="H45" s="6" t="s">
+      <c r="H51" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="I45" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="46" spans="2:9" ht="71.25" x14ac:dyDescent="0.25">
-      <c r="B46" s="3" t="s">
+      <c r="I51" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="52" spans="2:9" ht="57" x14ac:dyDescent="0.25">
+      <c r="B52" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="C46" s="6" t="s">
+      <c r="C52" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="D46" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E46" s="3" t="s">
+      <c r="D52" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E52" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="F46" s="3" t="s">
+      <c r="F52" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G46" s="3" t="s">
+      <c r="G52" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="H46" s="3" t="s">
+      <c r="H52" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="I46" s="19" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="47" spans="2:9" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="3" t="s">
+      <c r="I52" s="19" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="53" spans="2:9" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B53" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C47" s="6" t="s">
+      <c r="C53" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="D47" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="E47" s="3" t="s">
+      <c r="D53" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E53" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="F47" s="3" t="s">
+      <c r="F53" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="G47" s="3" t="s">
+      <c r="G53" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="H47" s="3" t="s">
+      <c r="H53" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="I47" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="48" spans="2:9" ht="57" x14ac:dyDescent="0.25">
-      <c r="B48" s="12" t="s">
+      <c r="I53" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="54" spans="2:9" ht="57" x14ac:dyDescent="0.25">
+      <c r="B54" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="C48" s="6" t="s">
+      <c r="C54" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="D48" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E48" s="12" t="s">
+      <c r="D54" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E54" s="12" t="s">
         <v>121</v>
       </c>
-      <c r="F48" s="12" t="s">
+      <c r="F54" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="G48" s="12" t="s">
+      <c r="G54" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="H48" s="17" t="s">
+      <c r="H54" s="17" t="s">
         <v>98</v>
       </c>
-      <c r="I48" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="49" spans="2:9" ht="57" x14ac:dyDescent="0.25">
-      <c r="B49" s="11" t="s">
+      <c r="I54" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="55" spans="2:9" ht="57" x14ac:dyDescent="0.25">
+      <c r="B55" s="11" t="s">
         <v>127</v>
       </c>
-      <c r="C49" s="10" t="s">
+      <c r="C55" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="D49" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="E49" s="11" t="s">
+      <c r="D55" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E55" s="11" t="s">
         <v>128</v>
       </c>
-      <c r="F49" s="11" t="s">
+      <c r="F55" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="G49" s="11" t="s">
+      <c r="G55" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="H49" s="11" t="s">
+      <c r="H55" s="11" t="s">
         <v>134</v>
       </c>
-      <c r="I49" s="11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="50" spans="2:9" ht="71.25" x14ac:dyDescent="0.25">
-      <c r="B50" s="12" t="s">
+      <c r="I55" s="11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="56" spans="2:9" ht="71.25" x14ac:dyDescent="0.25">
+      <c r="B56" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="C50" s="10" t="s">
+      <c r="C56" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="D50" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E50" s="16" t="s">
+      <c r="D56" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E56" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="F50" s="12" t="s">
+      <c r="F56" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="G50" s="12" t="s">
+      <c r="G56" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="H50" s="17" t="s">
+      <c r="H56" s="17" t="s">
         <v>103</v>
       </c>
-      <c r="I50" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="51" spans="2:9" ht="57" x14ac:dyDescent="0.25">
-      <c r="B51" s="12" t="s">
+      <c r="I56" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="57" spans="2:9" ht="57" x14ac:dyDescent="0.25">
+      <c r="B57" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="C51" s="10" t="s">
+      <c r="C57" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="D51" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E51" s="16" t="s">
+      <c r="D57" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E57" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="F51" s="12" t="s">
+      <c r="F57" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="G51" s="12" t="s">
+      <c r="G57" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="H51" s="17" t="s">
+      <c r="H57" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="I51" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="52" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="53" spans="2:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B53" s="23" t="s">
+      <c r="I57" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="58" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="59" spans="2:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B59" s="26" t="s">
         <v>107</v>
       </c>
-      <c r="C53" s="41"/>
-      <c r="D53" s="41"/>
-      <c r="E53" s="41"/>
-      <c r="F53" s="41"/>
-      <c r="G53" s="41"/>
-      <c r="H53" s="41"/>
-      <c r="I53" s="42"/>
-    </row>
-    <row r="54" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="22" t="s">
+      <c r="C59" s="27"/>
+      <c r="D59" s="27"/>
+      <c r="E59" s="27"/>
+      <c r="F59" s="27"/>
+      <c r="G59" s="27"/>
+      <c r="H59" s="27"/>
+      <c r="I59" s="28"/>
+    </row>
+    <row r="60" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B60" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C54" s="22" t="s">
+      <c r="C60" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="D54" s="22" t="s">
+      <c r="D60" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="E54" s="22" t="s">
+      <c r="E60" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="F54" s="22" t="s">
+      <c r="F60" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="G54" s="22" t="s">
+      <c r="G60" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="H54" s="22" t="s">
+      <c r="H60" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="I54" s="21" t="s">
+      <c r="I60" s="21" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="55" spans="2:9" ht="57" x14ac:dyDescent="0.25">
-      <c r="B55" s="6" t="s">
+    <row r="61" spans="2:9" ht="57" x14ac:dyDescent="0.25">
+      <c r="B61" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="C55" s="6" t="s">
+      <c r="C61" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="D55" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E55" s="6" t="s">
+      <c r="D61" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E61" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F55" s="6" t="s">
+      <c r="F61" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="G55" s="6" t="s">
+      <c r="G61" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="H55" s="6" t="s">
+      <c r="H61" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="I55" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="56" spans="2:9" ht="57" x14ac:dyDescent="0.25">
-      <c r="B56" s="3" t="s">
+      <c r="I61" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="62" spans="2:9" ht="57" x14ac:dyDescent="0.25">
+      <c r="B62" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="C56" s="6" t="s">
+      <c r="C62" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="D56" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E56" s="3" t="s">
+      <c r="D62" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E62" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="F56" s="3" t="s">
+      <c r="F62" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G56" s="3" t="s">
+      <c r="G62" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="H56" s="3" t="s">
+      <c r="H62" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="I56" s="43" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="57" spans="2:9" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="3" t="s">
+      <c r="I62" s="25" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="63" spans="2:9" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B63" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C57" s="6" t="s">
+      <c r="C63" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="D57" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="E57" s="3" t="s">
+      <c r="D63" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E63" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="F57" s="3" t="s">
+      <c r="F63" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="G57" s="3" t="s">
+      <c r="G63" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="H57" s="3" t="s">
+      <c r="H63" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="I57" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="58" spans="2:9" ht="71.25" x14ac:dyDescent="0.25">
-      <c r="B58" s="12" t="s">
+      <c r="I63" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="64" spans="2:9" ht="71.25" x14ac:dyDescent="0.25">
+      <c r="B64" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="C58" s="6" t="s">
+      <c r="C64" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="D58" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E58" s="3" t="s">
+      <c r="D64" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E64" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="F58" s="12" t="s">
+      <c r="F64" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="G58" s="12" t="s">
+      <c r="G64" s="12" t="s">
         <v>124</v>
       </c>
-      <c r="H58" s="12" t="s">
+      <c r="H64" s="12" t="s">
         <v>124</v>
       </c>
-      <c r="I58" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="59" spans="2:9" ht="57" x14ac:dyDescent="0.25">
-      <c r="B59" s="11" t="s">
+      <c r="I64" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="65" spans="2:9" ht="57" x14ac:dyDescent="0.25">
+      <c r="B65" s="11" t="s">
         <v>127</v>
       </c>
-      <c r="C59" s="10" t="s">
+      <c r="C65" s="10" t="s">
         <v>137</v>
       </c>
-      <c r="D59" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="E59" s="11" t="s">
+      <c r="D65" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E65" s="11" t="s">
         <v>128</v>
       </c>
-      <c r="F59" s="11" t="s">
+      <c r="F65" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="G59" s="11" t="s">
+      <c r="G65" s="11" t="s">
         <v>140</v>
       </c>
-      <c r="H59" s="11" t="s">
+      <c r="H65" s="11" t="s">
         <v>140</v>
       </c>
-      <c r="I59" s="11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="60" spans="2:9" ht="71.25" x14ac:dyDescent="0.25">
-      <c r="B60" s="12" t="s">
+      <c r="I65" s="11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="66" spans="2:9" ht="71.25" x14ac:dyDescent="0.25">
+      <c r="B66" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="C60" s="10" t="s">
+      <c r="C66" s="10" t="s">
         <v>138</v>
       </c>
-      <c r="D60" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E60" s="3" t="s">
+      <c r="D66" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E66" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="F60" s="12" t="s">
+      <c r="F66" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="G60" s="17" t="s">
+      <c r="G66" s="17" t="s">
         <v>125</v>
       </c>
-      <c r="H60" s="17" t="s">
+      <c r="H66" s="17" t="s">
         <v>125</v>
       </c>
-      <c r="I60" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="61" spans="2:9" ht="71.25" x14ac:dyDescent="0.25">
-      <c r="B61" s="12" t="s">
+      <c r="I66" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="67" spans="2:9" ht="71.25" x14ac:dyDescent="0.25">
+      <c r="B67" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="C61" s="10" t="s">
+      <c r="C67" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="D61" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E61" s="3" t="s">
+      <c r="D67" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E67" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="F61" s="12" t="s">
+      <c r="F67" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="G61" s="12" t="s">
+      <c r="G67" s="12" t="s">
         <v>126</v>
       </c>
-      <c r="H61" s="12" t="s">
+      <c r="H67" s="12" t="s">
         <v>126</v>
       </c>
-      <c r="I61" s="3" t="s">
+      <c r="I67" s="3" t="s">
         <v>10</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="39">
-    <mergeCell ref="B53:I53"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="H20:H21"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="G22:G23"/>
     <mergeCell ref="I17:I18"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="H14:H15"/>
     <mergeCell ref="D1:G1"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="G17:G18"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="G20:G21"/>
     <mergeCell ref="B8:I8"/>
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="D11:D12"/>
@@ -2612,22 +2803,23 @@
     <mergeCell ref="H11:H12"/>
     <mergeCell ref="I11:I12"/>
     <mergeCell ref="B11:B12"/>
-    <mergeCell ref="B43:I43"/>
     <mergeCell ref="B3:I3"/>
-    <mergeCell ref="B33:I33"/>
-    <mergeCell ref="B23:I23"/>
-    <mergeCell ref="H19:H20"/>
-    <mergeCell ref="I19:I20"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="F19:F20"/>
-    <mergeCell ref="G19:G20"/>
-    <mergeCell ref="I14:I15"/>
-    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="B59:I59"/>
+    <mergeCell ref="I20:I21"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="G17:G18"/>
     <mergeCell ref="H17:H18"/>
+    <mergeCell ref="B49:I49"/>
+    <mergeCell ref="B39:I39"/>
+    <mergeCell ref="B26:I26"/>
+    <mergeCell ref="H22:H23"/>
+    <mergeCell ref="I22:I23"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="C22:C23"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>